<commit_message>
added excel  output file
</commit_message>
<xml_diff>
--- a/file_comp/files/output.xlsx
+++ b/file_comp/files/output.xlsx
@@ -16,97 +16,97 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
   <si>
-    <t>16 #0000FF 16</t>
-  </si>
-  <si>
-    <t>2 #0000FF 2</t>
-  </si>
-  <si>
-    <t>50 #0000FF 50</t>
-  </si>
-  <si>
-    <t>12 #0000FF 12</t>
-  </si>
-  <si>
-    <t>deposits #0000FF deposits</t>
-  </si>
-  <si>
-    <t>deductions #0000FF deductions</t>
+    <t>16  16</t>
+  </si>
+  <si>
+    <t>2  2</t>
+  </si>
+  <si>
+    <t>50  50</t>
+  </si>
+  <si>
+    <t>12  12</t>
+  </si>
+  <si>
+    <t>deposits  deposits</t>
+  </si>
+  <si>
+    <t>deductions  deductions</t>
   </si>
   <si>
     <t>deposits</t>
   </si>
   <si>
-    <t>20 #0000FF 20</t>
-  </si>
-  <si>
-    <t>52 #0000FF 52</t>
-  </si>
-  <si>
-    <t>40 #0000FF 40</t>
-  </si>
-  <si>
-    <t>28 #0000FF 28</t>
-  </si>
-  <si>
-    <t>-8 #0000FF -8</t>
-  </si>
-  <si>
-    <t>-20 #0000FF -20</t>
-  </si>
-  <si>
-    <t>-56 #0000FF -56</t>
-  </si>
-  <si>
-    <t>-80 #0000FF -80</t>
-  </si>
-  <si>
-    <t>-92 #0000FF -92</t>
-  </si>
-  <si>
-    <t>-104 #0000FF -104</t>
-  </si>
-  <si>
-    <t>2020-12-01 14:30:40 #0000FF 2020-12-01 14:30:40</t>
-  </si>
-  <si>
-    <t>2021-02-03 14:38:19 #0000FF 2021-02-03 14:38:19</t>
-  </si>
-  <si>
-    <t>2020-12-02 10:00:03 #0000FF 2020-12-02 10:00:03</t>
-  </si>
-  <si>
-    <t>2020-12-10 10:30:38 #0000FF 2020-12-10 10:30:38</t>
-  </si>
-  <si>
-    <t>2020-12-17 10:00:02 #0000FF 2020-12-17 10:00:02</t>
-  </si>
-  <si>
-    <t>2020-12-24 10:00:03 #0000FF 2020-12-24 10:00:03</t>
-  </si>
-  <si>
-    <t>2020-12-31 10:00:02 #0000FF 2020-12-31 10:00:02</t>
-  </si>
-  <si>
-    <t>2021-01-07 10:00:03 #0000FF 2021-01-07 10:00:03</t>
-  </si>
-  <si>
-    <t>2021-01-14 10:00:03 #0000FF 2021-01-14 10:00:03</t>
-  </si>
-  <si>
-    <t>2021-01-21 10:00:03 #0000FF 2021-01-21 10:00:03</t>
-  </si>
-  <si>
-    <t>2021-01-28 10:00:02 #0000FF 2021-01-28 10:00:02</t>
-  </si>
-  <si>
-    <t>2021-02-04 10:00:02 #0000FF 2021-02-04 10:00:02</t>
-  </si>
-  <si>
-    <t>2021-02-11 10:00:06 #0000FF 2021-02-11 10:00:06</t>
-  </si>
-  <si>
-    <t>2021-02-18 10:00:06 #0000FF 2021-02-18 10:00:06</t>
+    <t>20  20</t>
+  </si>
+  <si>
+    <t>52  52</t>
+  </si>
+  <si>
+    <t>40  40</t>
+  </si>
+  <si>
+    <t>28  28</t>
+  </si>
+  <si>
+    <t>-8  -8</t>
+  </si>
+  <si>
+    <t>-20  -20</t>
+  </si>
+  <si>
+    <t>-56  -56</t>
+  </si>
+  <si>
+    <t>-80  -80</t>
+  </si>
+  <si>
+    <t>-92  -92</t>
+  </si>
+  <si>
+    <t>-104  -104</t>
+  </si>
+  <si>
+    <t>2020-12-01 14:30:40  2020-12-01 14:30:40</t>
+  </si>
+  <si>
+    <t>2021-02-03 14:38:19  2021-02-03 14:38:19</t>
+  </si>
+  <si>
+    <t>2020-12-02 10:00:03  2020-12-02 10:00:03</t>
+  </si>
+  <si>
+    <t>2020-12-10 10:30:38  2020-12-10 10:30:38</t>
+  </si>
+  <si>
+    <t>2020-12-17 10:00:02  2020-12-17 10:00:02</t>
+  </si>
+  <si>
+    <t>2020-12-24 10:00:03  2020-12-24 10:00:03</t>
+  </si>
+  <si>
+    <t>2020-12-31 10:00:02  2020-12-31 10:00:02</t>
+  </si>
+  <si>
+    <t>2021-01-07 10:00:03  2021-01-07 10:00:03</t>
+  </si>
+  <si>
+    <t>2021-01-14 10:00:03  2021-01-14 10:00:03</t>
+  </si>
+  <si>
+    <t>2021-01-21 10:00:03  2021-01-21 10:00:03</t>
+  </si>
+  <si>
+    <t>2021-01-28 10:00:02  2021-01-28 10:00:02</t>
+  </si>
+  <si>
+    <t>2021-02-04 10:00:02  2021-02-04 10:00:02</t>
+  </si>
+  <si>
+    <t>2021-02-11 10:00:06  2021-02-11 10:00:06</t>
+  </si>
+  <si>
+    <t>2021-02-18 10:00:06  2021-02-18 10:00:06</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
completed working on  highlight duplicatesfunctionality file that highlight all duplicates
</commit_message>
<xml_diff>
--- a/file_comp/files/output.xlsx
+++ b/file_comp/files/output.xlsx
@@ -374,7 +374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,6 +402,26 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
         <v>50</v>
       </c>
     </row>

</xml_diff>